<commit_message>
fixed bug in EGW props, add differential sensors, removed outer environment where unneccessary
</commit_message>
<xml_diff>
--- a/Media/data/Dynalene Ethylene Glycol.xlsx
+++ b/Media/data/Dynalene Ethylene Glycol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Projects\ModelicaProjects\DynTherM\Media\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BBF028-FB72-4182-8F0F-F0BE6E8401FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429E47AC-653E-4294-9CCC-1E7B8C3258F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{32BF7C39-58A3-4B4A-A775-0F246D126BDC}"/>
+    <workbookView xWindow="14565" yWindow="-21600" windowWidth="26010" windowHeight="20985" activeTab="3" xr2:uid="{32BF7C39-58A3-4B4A-A775-0F246D126BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="viscosity" sheetId="1" r:id="rId1"/>
@@ -10251,12 +10251,12 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -10318,7 +10318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -10382,7 +10382,7 @@
         <v>8.9700000000000002E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-20</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>6.0499999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -10514,7 +10514,7 @@
         <v>4.2100000000000005E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -10582,7 +10582,7 @@
         <v>3.0100000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10</v>
       </c>
@@ -10652,7 +10652,7 @@
         <v>2.2100000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20</v>
       </c>
@@ -10724,7 +10724,7 @@
         <v>1.66E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>40</v>
       </c>
@@ -10868,7 +10868,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50</v>
       </c>
@@ -10940,7 +10940,7 @@
         <v>7.8499999999999993E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>60</v>
       </c>
@@ -11012,7 +11012,7 @@
         <v>6.3300000000000006E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>70</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>5.1700000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>80</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>4.28E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>90</v>
       </c>
@@ -11228,7 +11228,7 @@
         <v>3.5800000000000003E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>100</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>3.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>120</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>2.2300000000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>140</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>1.6899999999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>1.32E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180</v>
       </c>
@@ -11588,7 +11588,7 @@
         <v>1.0600000000000002E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>200</v>
       </c>
@@ -11660,7 +11660,7 @@
         <v>8.5999999999999998E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>220</v>
       </c>
@@ -11746,14 +11746,14 @@
       <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -11879,7 +11879,7 @@
         <v>2800.4340000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-20</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>2821.364</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -12011,7 +12011,7 @@
         <v>2846.48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -12079,7 +12079,7 @@
         <v>2871.596</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10</v>
       </c>
@@ -12149,7 +12149,7 @@
         <v>2896.712</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>2921.828</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
@@ -12293,7 +12293,7 @@
         <v>2946.944</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>40</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>2972.06</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>2997.1759999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>60</v>
       </c>
@@ -12509,7 +12509,7 @@
         <v>3022.2919999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>70</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>3047.4079999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>80</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>3072.5239999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>90</v>
       </c>
@@ -12725,7 +12725,7 @@
         <v>3097.64</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>100</v>
       </c>
@@ -12797,7 +12797,7 @@
         <v>3122.7559999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>120</v>
       </c>
@@ -12869,7 +12869,7 @@
         <v>3168.8020000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>140</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>3219.0340000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -13013,7 +13013,7 @@
         <v>3269.2660000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>3319.498</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>200</v>
       </c>
@@ -13157,7 +13157,7 @@
         <v>3369.73</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>220</v>
       </c>
@@ -13243,14 +13243,14 @@
       <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="13" max="21" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -13312,7 +13312,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -13376,7 +13376,7 @@
         <v>1126.4000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-20</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>1124.1600000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>1121.5999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -13576,7 +13576,7 @@
         <v>1119.04</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>1116.48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>1113.5999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
@@ -13790,7 +13790,7 @@
         <v>1110.8800000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>40</v>
       </c>
@@ -13862,7 +13862,7 @@
         <v>1107.8399999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50</v>
       </c>
@@ -13934,7 +13934,7 @@
         <v>1105.28</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>60</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>1101.76</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>70</v>
       </c>
@@ -14078,7 +14078,7 @@
         <v>1098.56</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>80</v>
       </c>
@@ -14150,7 +14150,7 @@
         <v>1095.3599999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>90</v>
       </c>
@@ -14222,7 +14222,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>100</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>1088.48</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>120</v>
       </c>
@@ -14366,7 +14366,7 @@
         <v>1081.28</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>140</v>
       </c>
@@ -14438,7 +14438,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -14510,7 +14510,7 @@
         <v>1065.76</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180</v>
       </c>
@@ -14582,7 +14582,7 @@
         <v>1057.44</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>200</v>
       </c>
@@ -14654,7 +14654,7 @@
         <v>1048.6400000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>220</v>
       </c>
@@ -14736,17 +14736,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56E54B9-D7DB-458B-AAA4-B5625854FCA0}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="21" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>55</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>-30</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>0.30806459999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>-20</v>
       </c>
@@ -14938,7 +14938,7 @@
         <v>0.3132567</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>-10</v>
       </c>
@@ -15004,7 +15004,7 @@
         <v>0.31844879999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -15072,7 +15072,7 @@
         <v>0.32191019999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>0.32710229999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>20</v>
       </c>
@@ -15214,7 +15214,7 @@
         <v>0.33056369999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
@@ -15286,7 +15286,7 @@
         <v>0.33575579999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>40</v>
       </c>
@@ -15358,7 +15358,7 @@
         <v>0.3392172</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>50</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>0.3426786</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>60</v>
       </c>
@@ -15502,7 +15502,7 @@
         <v>0.34614</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>70</v>
       </c>
@@ -15574,7 +15574,7 @@
         <v>0.34960140000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>80</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>0.35306279999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>90</v>
       </c>
@@ -15718,7 +15718,7 @@
         <v>0.35652419999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>100</v>
       </c>
@@ -15790,7 +15790,7 @@
         <v>0.35998559999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>120</v>
       </c>
@@ -15862,7 +15862,7 @@
         <v>0.36344699999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>140</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>0.3686391</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -16006,7 +16006,7 @@
         <v>0.3721005</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180</v>
       </c>
@@ -16078,7 +16078,7 @@
         <v>0.3755619</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>200</v>
       </c>
@@ -16150,7 +16150,7 @@
         <v>0.37729259999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>220</v>
       </c>

</xml_diff>